<commit_message>
Add cmt-studentify reference documentation
- Update cmt-mainadm
- Add cmt-reference section
- Update cmt-studentify
- Add various cross-links
</commit_message>
<xml_diff>
--- a/images/cmt-mainadm-samples-for-documentation purposes.xlsx
+++ b/images/cmt-mainadm-samples-for-documentation purposes.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericloots/Trainingen/LBT/course-management-tools/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E830C51-FC82-EC46-9143-391EDB6A16E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433A4B21-9805-5F46-B1E3-0598CE8992B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6860" yWindow="3080" windowWidth="27640" windowHeight="16940" activeTab="4" xr2:uid="{E7404945-19DE-8A45-9D99-DC02C4AA41DE}"/>
+    <workbookView xWindow="6860" yWindow="3080" windowWidth="27640" windowHeight="16940" activeTab="5" xr2:uid="{E7404945-19DE-8A45-9D99-DC02C4AA41DE}"/>
   </bookViews>
   <sheets>
     <sheet name="DIB renum" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Renumber offset&amp;stepsize" sheetId="3" r:id="rId3"/>
     <sheet name="Renumber stepsize" sheetId="4" r:id="rId4"/>
     <sheet name="Renumber offset" sheetId="5" r:id="rId5"/>
+    <sheet name="Renumber offset (2)" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="50">
   <si>
     <t>exercise_000_sudoku_solver_initial_state</t>
   </si>
@@ -164,6 +165,21 @@
   </si>
   <si>
     <t>exercise_017_givens</t>
+  </si>
+  <si>
+    <t>exercise_008_enum_and_export</t>
+  </si>
+  <si>
+    <t>exercise_009_union_types</t>
+  </si>
+  <si>
+    <t>exercise_010_opaque_type_aliases</t>
+  </si>
+  <si>
+    <t>exercise_011_multiversal_equality</t>
+  </si>
+  <si>
+    <t>Exercises</t>
   </si>
 </sst>
 </file>
@@ -256,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -265,6 +281,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,6 +601,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{504A8F23-01EA-CF40-A12B-EA96AE36C570}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
@@ -676,6 +699,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DECA936E-3E97-9D48-B660-6C133383519B}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
@@ -773,6 +797,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0008B3-742B-4B41-A34D-0F9F83CF8DA1}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
@@ -868,6 +893,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E39804A-B7AB-064A-9D32-506A1255669C}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
@@ -963,9 +989,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9B2A799-5834-E040-AD75-203318331426}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="B2:C11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1054,4 +1081,99 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF09567E-6C80-8D4C-9F46-756AA86F8009}">
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="B2:C14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" customWidth="1"/>
+    <col min="2" max="3" width="62.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="17">
+      <c r="B2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="2:3" ht="17">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="2:3" ht="17">
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="2:3" ht="17">
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="2:3" ht="17">
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="2:3" ht="17">
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="2:3" ht="17">
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="2:3" ht="17">
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="2:3" ht="17">
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="2:3" ht="17">
+      <c r="B11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="2:3" ht="17">
+      <c r="B12" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="17">
+      <c r="B13" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="17">
+      <c r="B14" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add cmt-studentify reference documentation (#130)
- Update cmt-mainadm
- Add cmt-reference section
- Update cmt-studentify
- Add various cross-links
</commit_message>
<xml_diff>
--- a/images/cmt-mainadm-samples-for-documentation purposes.xlsx
+++ b/images/cmt-mainadm-samples-for-documentation purposes.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericloots/Trainingen/LBT/course-management-tools/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E830C51-FC82-EC46-9143-391EDB6A16E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433A4B21-9805-5F46-B1E3-0598CE8992B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6860" yWindow="3080" windowWidth="27640" windowHeight="16940" activeTab="4" xr2:uid="{E7404945-19DE-8A45-9D99-DC02C4AA41DE}"/>
+    <workbookView xWindow="6860" yWindow="3080" windowWidth="27640" windowHeight="16940" activeTab="5" xr2:uid="{E7404945-19DE-8A45-9D99-DC02C4AA41DE}"/>
   </bookViews>
   <sheets>
     <sheet name="DIB renum" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Renumber offset&amp;stepsize" sheetId="3" r:id="rId3"/>
     <sheet name="Renumber stepsize" sheetId="4" r:id="rId4"/>
     <sheet name="Renumber offset" sheetId="5" r:id="rId5"/>
+    <sheet name="Renumber offset (2)" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="50">
   <si>
     <t>exercise_000_sudoku_solver_initial_state</t>
   </si>
@@ -164,6 +165,21 @@
   </si>
   <si>
     <t>exercise_017_givens</t>
+  </si>
+  <si>
+    <t>exercise_008_enum_and_export</t>
+  </si>
+  <si>
+    <t>exercise_009_union_types</t>
+  </si>
+  <si>
+    <t>exercise_010_opaque_type_aliases</t>
+  </si>
+  <si>
+    <t>exercise_011_multiversal_equality</t>
+  </si>
+  <si>
+    <t>Exercises</t>
   </si>
 </sst>
 </file>
@@ -256,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -265,6 +281,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,6 +601,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{504A8F23-01EA-CF40-A12B-EA96AE36C570}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
@@ -676,6 +699,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DECA936E-3E97-9D48-B660-6C133383519B}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
@@ -773,6 +797,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0008B3-742B-4B41-A34D-0F9F83CF8DA1}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
@@ -868,6 +893,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E39804A-B7AB-064A-9D32-506A1255669C}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
@@ -963,9 +989,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9B2A799-5834-E040-AD75-203318331426}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="B2:C11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1054,4 +1081,99 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF09567E-6C80-8D4C-9F46-756AA86F8009}">
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="B2:C14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" customWidth="1"/>
+    <col min="2" max="3" width="62.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="17">
+      <c r="B2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="2:3" ht="17">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="2:3" ht="17">
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="2:3" ht="17">
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="2:3" ht="17">
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="2:3" ht="17">
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="2:3" ht="17">
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="2:3" ht="17">
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="2:3" ht="17">
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="2:3" ht="17">
+      <c r="B11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="2:3" ht="17">
+      <c r="B12" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="17">
+      <c r="B13" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="17">
+      <c r="B14" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>